<commit_message>
example 3 solution pdf
</commit_message>
<xml_diff>
--- a/Zadani_3.xlsx
+++ b/Zadani_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mefit\Documents\gamba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF973B8-BE53-42D0-9AD1-C01FCF9A4BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E42C64-D6EC-4C05-9265-852E644E54E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,12 +93,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{46F29295-1624-4730-8B40-5938A6171606}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>Matěj Černohous:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+WILD SYMBOL</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Symbol</t>
   </si>
@@ -167,12 +193,18 @@
   </si>
   <si>
     <t>Bonusová hra</t>
+  </si>
+  <si>
+    <t>Frekvence hitů</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -287,15 +319,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -331,6 +360,12 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,10 +382,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -616,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S23"/>
+  <dimension ref="B2:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.3"/>
@@ -641,30 +672,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>5</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="12">
         <v>2</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B3" s="7"/>
-      <c r="E3" s="9"/>
+      <c r="B3" s="6"/>
+      <c r="E3" s="8"/>
       <c r="H3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <v>2000</v>
       </c>
     </row>
@@ -672,29 +703,29 @@
       <c r="H4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <v>4330</v>
       </c>
     </row>
     <row r="6" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="G6" s="4" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="G6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="M6" s="4" t="s">
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="M6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
     </row>
     <row r="7" spans="2:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
@@ -734,61 +765,61 @@
       <c r="P7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="S7" s="4"/>
+      <c r="S7" s="14"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>0</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>9</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <f>C8</f>
         <v>9</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>8</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <f>C8*D8*E8*$C$2</f>
         <v>3240</v>
       </c>
-      <c r="H8" s="8">
-        <f>(C8*D8*$E$16+C8*$D$16*E8+$C$16*D8*E8)*$C$2</f>
+      <c r="H8" s="7">
+        <f t="shared" ref="H8:H15" si="0">(C8*D8*$E$16+C8*$D$16*E8+$C$16*D8*E8)*$C$2</f>
         <v>1125</v>
       </c>
-      <c r="I8" s="8">
-        <f>(C8*$D$16*$E$16+D8*$C$16*$E$16+E8*$C$16*$D$16)*$C$2</f>
+      <c r="I8" s="7">
+        <f t="shared" ref="I8:I15" si="1">(C8*$D$16*$E$16+D8*$C$16*$E$16+E8*$C$16*$D$16)*$C$2</f>
         <v>130</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="4"/>
       <c r="K8" s="1">
         <v>2</v>
       </c>
-      <c r="M8" s="10">
-        <f>(G8*$K8)/($C$18*$F$2)</f>
+      <c r="M8" s="9">
+        <f t="shared" ref="M8:M16" si="2">(G8*$K8)/($C$18*$F$2)</f>
         <v>7.7791116446578629E-2</v>
       </c>
-      <c r="N8" s="10">
-        <f>(H8*$K8*2)/($C$18*$F$2)</f>
+      <c r="N8" s="9">
+        <f t="shared" ref="N8:N15" si="3">(H8*$K8*2)/($C$18*$F$2)</f>
         <v>5.4021608643457383E-2</v>
       </c>
-      <c r="O8" s="10">
-        <f>(I8*$K8*4)/($C$18*$F$2)</f>
+      <c r="O8" s="9">
+        <f t="shared" ref="O8:O15" si="4">(I8*$K8*4)/($C$18*$F$2)</f>
         <v>1.248499399759904E-2</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="9">
         <f>SUM(M8:O8)</f>
         <v>0.14429771908763503</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="S8" s="14">
+      <c r="S8" s="13">
         <f>SUM(P8:P15)/P16</f>
         <v>0.80002527326720163</v>
       </c>
@@ -797,53 +828,53 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <v>6</v>
       </c>
-      <c r="D9" s="13">
-        <f t="shared" ref="D9:E9" si="0">C9</f>
+      <c r="D9" s="12">
+        <f t="shared" ref="D9:E9" si="5">C9</f>
         <v>6</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" ref="G9:G16" si="6">C9*D9*E9*$C$2</f>
+        <v>1080</v>
+      </c>
+      <c r="H9" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G9" s="8">
-        <f t="shared" ref="G9:G16" si="1">C9*D9*E9*$C$2</f>
-        <v>1080</v>
-      </c>
-      <c r="H9" s="8">
-        <f>(C9*D9*$E$16+C9*$D$16*E9+$C$16*D9*E9)*$C$2</f>
         <v>540</v>
       </c>
-      <c r="I9" s="8">
-        <f>(C9*$D$16*$E$16+D9*$C$16*$E$16+E9*$C$16*$D$16)*$C$2</f>
+      <c r="I9" s="7">
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="4"/>
       <c r="K9" s="1">
         <v>2</v>
       </c>
-      <c r="M9" s="10">
-        <f>(G9*$K9)/($C$18*$F$2)</f>
+      <c r="M9" s="9">
+        <f t="shared" si="2"/>
         <v>2.5930372148859543E-2</v>
       </c>
-      <c r="N9" s="10">
-        <f>(H9*$K9*2)/($C$18*$F$2)</f>
+      <c r="N9" s="9">
+        <f t="shared" si="3"/>
         <v>2.5930372148859543E-2</v>
       </c>
-      <c r="O9" s="10">
-        <f>(I9*$K9*4)/($C$18*$F$2)</f>
+      <c r="O9" s="9">
+        <f t="shared" si="4"/>
         <v>8.6434573829531815E-3</v>
       </c>
-      <c r="P9" s="10">
-        <f t="shared" ref="P9:P15" si="2">SUM(M9:O9)</f>
+      <c r="P9" s="9">
+        <f t="shared" ref="P9:P15" si="7">SUM(M9:O9)</f>
         <v>6.0504201680672269E-2</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S9" s="14">
+      <c r="S9" s="13">
         <f>M16/P16</f>
         <v>0.19997472673279837</v>
       </c>
@@ -852,47 +883,47 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>4</v>
       </c>
-      <c r="D10" s="13">
-        <f t="shared" ref="D10:E10" si="3">C10</f>
+      <c r="D10" s="12">
+        <f t="shared" ref="D10:E10" si="8">C10</f>
         <v>4</v>
       </c>
-      <c r="E10" s="13">
-        <f t="shared" si="3"/>
+      <c r="E10" s="12">
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
+        <f t="shared" si="6"/>
+        <v>320</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="I10" s="7">
         <f t="shared" si="1"/>
-        <v>320</v>
-      </c>
-      <c r="H10" s="8">
-        <f>(C10*D10*$E$16+C10*$D$16*E10+$C$16*D10*E10)*$C$2</f>
-        <v>240</v>
-      </c>
-      <c r="I10" s="8">
-        <f>(C10*$D$16*$E$16+D10*$C$16*$E$16+E10*$C$16*$D$16)*$C$2</f>
         <v>60</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="J10" s="4"/>
       <c r="K10" s="1">
         <v>5</v>
       </c>
-      <c r="M10" s="10">
-        <f>(G10*$K10)/($C$18*$F$2)</f>
+      <c r="M10" s="9">
+        <f t="shared" si="2"/>
         <v>1.920768307322929E-2</v>
       </c>
-      <c r="N10" s="10">
-        <f>(H10*$K10*2)/($C$18*$F$2)</f>
+      <c r="N10" s="9">
+        <f t="shared" si="3"/>
         <v>2.8811524609843937E-2</v>
       </c>
-      <c r="O10" s="10">
-        <f>(I10*$K10*4)/($C$18*$F$2)</f>
+      <c r="O10" s="9">
+        <f t="shared" si="4"/>
         <v>1.4405762304921969E-2</v>
       </c>
-      <c r="P10" s="10">
-        <f t="shared" si="2"/>
+      <c r="P10" s="9">
+        <f t="shared" si="7"/>
         <v>6.2424969987995196E-2</v>
       </c>
     </row>
@@ -900,46 +931,46 @@
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="12">
         <v>4</v>
       </c>
-      <c r="D11" s="13">
-        <f t="shared" ref="D11:E11" si="4">C11</f>
+      <c r="D11" s="12">
+        <f t="shared" ref="D11" si="9">C11</f>
         <v>4</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <v>4</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
+        <f t="shared" si="6"/>
+        <v>320</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="I11" s="7">
         <f t="shared" si="1"/>
-        <v>320</v>
-      </c>
-      <c r="H11" s="8">
-        <f>(C11*D11*$E$16+C11*$D$16*E11+$C$16*D11*E11)*$C$2</f>
-        <v>240</v>
-      </c>
-      <c r="I11" s="8">
-        <f>(C11*$D$16*$E$16+D11*$C$16*$E$16+E11*$C$16*$D$16)*$C$2</f>
         <v>60</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="J11" s="4"/>
       <c r="K11" s="1">
         <v>5</v>
       </c>
-      <c r="M11" s="10">
-        <f>(G11*$K11)/($C$18*$F$2)</f>
+      <c r="M11" s="9">
+        <f t="shared" si="2"/>
         <v>1.920768307322929E-2</v>
       </c>
-      <c r="N11" s="10">
-        <f>(H11*$K11*2)/($C$18*$F$2)</f>
+      <c r="N11" s="9">
+        <f t="shared" si="3"/>
         <v>2.8811524609843937E-2</v>
       </c>
-      <c r="O11" s="10">
-        <f>(I11*$K11*4)/($C$18*$F$2)</f>
+      <c r="O11" s="9">
+        <f t="shared" si="4"/>
         <v>1.4405762304921969E-2</v>
       </c>
-      <c r="P11" s="10">
-        <f t="shared" si="2"/>
+      <c r="P11" s="9">
+        <f t="shared" si="7"/>
         <v>6.2424969987995196E-2</v>
       </c>
     </row>
@@ -947,46 +978,46 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="12">
         <v>4</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <v>4</v>
       </c>
-      <c r="E12" s="13">
-        <f t="shared" ref="D12:E12" si="5">D12</f>
+      <c r="E12" s="12">
+        <f t="shared" ref="E12" si="10">D12</f>
         <v>4</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
+        <f t="shared" si="6"/>
+        <v>320</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="I12" s="7">
         <f t="shared" si="1"/>
-        <v>320</v>
-      </c>
-      <c r="H12" s="8">
-        <f>(C12*D12*$E$16+C12*$D$16*E12+$C$16*D12*E12)*$C$2</f>
-        <v>240</v>
-      </c>
-      <c r="I12" s="8">
-        <f>(C12*$D$16*$E$16+D12*$C$16*$E$16+E12*$C$16*$D$16)*$C$2</f>
         <v>60</v>
       </c>
-      <c r="J12" s="5"/>
+      <c r="J12" s="4"/>
       <c r="K12" s="1">
         <v>10</v>
       </c>
-      <c r="M12" s="10">
-        <f>(G12*$K12)/($C$18*$F$2)</f>
+      <c r="M12" s="9">
+        <f t="shared" si="2"/>
         <v>3.8415366146458581E-2</v>
       </c>
-      <c r="N12" s="10">
-        <f>(H12*$K12*2)/($C$18*$F$2)</f>
+      <c r="N12" s="9">
+        <f t="shared" si="3"/>
         <v>5.7623049219687875E-2</v>
       </c>
-      <c r="O12" s="10">
-        <f>(I12*$K12*4)/($C$18*$F$2)</f>
+      <c r="O12" s="9">
+        <f t="shared" si="4"/>
         <v>2.8811524609843937E-2</v>
       </c>
-      <c r="P12" s="10">
-        <f t="shared" si="2"/>
+      <c r="P12" s="9">
+        <f t="shared" si="7"/>
         <v>0.12484993997599039</v>
       </c>
     </row>
@@ -994,47 +1025,47 @@
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="12">
         <v>3</v>
       </c>
-      <c r="D13" s="13">
-        <f t="shared" ref="D13:E13" si="6">C13</f>
+      <c r="D13" s="12">
+        <f t="shared" ref="D13:E13" si="11">C13</f>
         <v>3</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="G13" s="7">
         <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="G13" s="8">
+        <v>135</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="I13" s="7">
         <f t="shared" si="1"/>
-        <v>135</v>
-      </c>
-      <c r="H13" s="8">
-        <f>(C13*D13*$E$16+C13*$D$16*E13+$C$16*D13*E13)*$C$2</f>
-        <v>135</v>
-      </c>
-      <c r="I13" s="8">
-        <f>(C13*$D$16*$E$16+D13*$C$16*$E$16+E13*$C$16*$D$16)*$C$2</f>
         <v>45</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="J13" s="4"/>
       <c r="K13" s="1">
         <v>10</v>
       </c>
-      <c r="M13" s="10">
-        <f>(G13*$K13)/($C$18*$F$2)</f>
+      <c r="M13" s="9">
+        <f t="shared" si="2"/>
         <v>1.6206482593037214E-2</v>
       </c>
-      <c r="N13" s="10">
-        <f>(H13*$K13*2)/($C$18*$F$2)</f>
+      <c r="N13" s="9">
+        <f t="shared" si="3"/>
         <v>3.2412965186074429E-2</v>
       </c>
-      <c r="O13" s="10">
-        <f>(I13*$K13*4)/($C$18*$F$2)</f>
+      <c r="O13" s="9">
+        <f t="shared" si="4"/>
         <v>2.1608643457382955E-2</v>
       </c>
-      <c r="P13" s="10">
-        <f t="shared" si="2"/>
+      <c r="P13" s="9">
+        <f t="shared" si="7"/>
         <v>7.0228091236494594E-2</v>
       </c>
     </row>
@@ -1042,46 +1073,46 @@
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <v>2</v>
       </c>
-      <c r="D14" s="13">
-        <f t="shared" ref="D14:E14" si="7">C14</f>
+      <c r="D14" s="12">
+        <f t="shared" ref="D14" si="12">C14</f>
         <v>2</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>2</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="I14" s="7">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="H14" s="8">
-        <f>(C14*D14*$E$16+C14*$D$16*E14+$C$16*D14*E14)*$C$2</f>
-        <v>60</v>
-      </c>
-      <c r="I14" s="8">
-        <f>(C14*$D$16*$E$16+D14*$C$16*$E$16+E14*$C$16*$D$16)*$C$2</f>
         <v>30</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="J14" s="4"/>
       <c r="K14" s="1">
         <v>20</v>
       </c>
-      <c r="M14" s="10">
-        <f>(G14*$K14)/($C$18*$F$2)</f>
+      <c r="M14" s="9">
+        <f t="shared" si="2"/>
         <v>9.6038415366146452E-3</v>
       </c>
-      <c r="N14" s="10">
-        <f>(H14*$K14*2)/($C$18*$F$2)</f>
+      <c r="N14" s="9">
+        <f t="shared" si="3"/>
         <v>2.8811524609843937E-2</v>
       </c>
-      <c r="O14" s="10">
-        <f>(I14*$K14*4)/($C$18*$F$2)</f>
+      <c r="O14" s="9">
+        <f t="shared" si="4"/>
         <v>2.8811524609843937E-2</v>
       </c>
-      <c r="P14" s="10">
-        <f t="shared" si="2"/>
+      <c r="P14" s="9">
+        <f t="shared" si="7"/>
         <v>6.7226890756302518E-2</v>
       </c>
     </row>
@@ -1089,45 +1120,45 @@
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="12">
         <v>2</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="12">
         <v>2</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <v>2</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="I15" s="7">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="H15" s="8">
-        <f>(C15*D15*$E$16+C15*$D$16*E15+$C$16*D15*E15)*$C$2</f>
-        <v>60</v>
-      </c>
-      <c r="I15" s="8">
-        <f>(C15*$D$16*$E$16+D15*$C$16*$E$16+E15*$C$16*$D$16)*$C$2</f>
         <v>30</v>
       </c>
-      <c r="J15" s="5"/>
+      <c r="J15" s="4"/>
       <c r="K15" s="1">
         <v>50</v>
       </c>
-      <c r="M15" s="10">
-        <f>(G15*$K15)/($C$18*$F$2)</f>
+      <c r="M15" s="9">
+        <f t="shared" si="2"/>
         <v>2.4009603841536616E-2</v>
       </c>
-      <c r="N15" s="10">
-        <f>(H15*$K15*2)/($C$18*$F$2)</f>
+      <c r="N15" s="9">
+        <f t="shared" si="3"/>
         <v>7.202881152460984E-2</v>
       </c>
-      <c r="O15" s="10">
-        <f>(I15*$K15*4)/($C$18*$F$2)</f>
+      <c r="O15" s="9">
+        <f t="shared" si="4"/>
         <v>7.202881152460984E-2</v>
       </c>
-      <c r="P15" s="10">
-        <f t="shared" si="2"/>
+      <c r="P15" s="9">
+        <f t="shared" si="7"/>
         <v>0.16806722689075632</v>
       </c>
     </row>
@@ -1135,37 +1166,37 @@
       <c r="B16" s="2">
         <v>8</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="12">
         <v>1</v>
       </c>
-      <c r="D16" s="13">
-        <f t="shared" ref="D16:E16" si="8">C16</f>
+      <c r="D16" s="12">
+        <f t="shared" ref="D16:E16" si="13">C16</f>
         <v>1</v>
       </c>
-      <c r="E16" s="13">
-        <f t="shared" si="8"/>
+      <c r="E16" s="12">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="G16" s="8">
-        <f t="shared" si="1"/>
+      <c r="G16" s="7">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="5"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="4"/>
       <c r="K16" s="2">
         <f>(I3+I4)/2</f>
         <v>3165</v>
       </c>
-      <c r="M16" s="10">
-        <f>(G16*$K16)/($C$18*$F$2)</f>
+      <c r="M16" s="9">
+        <f t="shared" si="2"/>
         <v>0.18997599039615845</v>
       </c>
-      <c r="N16" s="10"/>
-      <c r="O16" s="11" t="s">
+      <c r="N16" s="9"/>
+      <c r="O16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="12">
+      <c r="P16" s="11">
         <f>SUM(P8:P15)+M16</f>
         <v>0.95</v>
       </c>
@@ -1179,11 +1210,11 @@
         <v>35</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" ref="D17:E17" si="9">SUM(D8:D16)</f>
+        <f t="shared" ref="D17:E17" si="14">SUM(D8:D16)</f>
         <v>35</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>34</v>
       </c>
     </row>
@@ -1197,19 +1228,19 @@
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G19" s="8"/>
-      <c r="H19" s="10"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="2:16" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G21" s="3"/>
@@ -1223,34 +1254,193 @@
       <c r="P21" s="3"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="5"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="G22" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="4"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="5"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
+      <c r="F23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
+        <f>G8/$C$18</f>
+        <v>7.7791116446578629E-2</v>
+      </c>
+      <c r="H24" s="9">
+        <f t="shared" ref="H24:I24" si="15">H8/$C$18</f>
+        <v>2.7010804321728692E-2</v>
+      </c>
+      <c r="I24" s="9">
+        <f t="shared" si="15"/>
+        <v>3.1212484993997599E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" ref="G25:I25" si="16">G9/$C$18</f>
+        <v>2.5930372148859543E-2</v>
+      </c>
+      <c r="H25" s="9">
+        <f t="shared" si="16"/>
+        <v>1.2965186074429771E-2</v>
+      </c>
+      <c r="I25" s="9">
+        <f t="shared" si="16"/>
+        <v>2.1608643457382954E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F26" s="3">
+        <v>2</v>
+      </c>
+      <c r="G26" s="9">
+        <f t="shared" ref="G26:I26" si="17">G10/$C$18</f>
+        <v>7.683073229291717E-3</v>
+      </c>
+      <c r="H26" s="9">
+        <f t="shared" si="17"/>
+        <v>5.7623049219687871E-3</v>
+      </c>
+      <c r="I26" s="9">
+        <f t="shared" si="17"/>
+        <v>1.4405762304921968E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F27" s="3">
+        <v>3</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" ref="G27:I27" si="18">G11/$C$18</f>
+        <v>7.683073229291717E-3</v>
+      </c>
+      <c r="H27" s="9">
+        <f t="shared" si="18"/>
+        <v>5.7623049219687871E-3</v>
+      </c>
+      <c r="I27" s="9">
+        <f t="shared" si="18"/>
+        <v>1.4405762304921968E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F28" s="3">
+        <v>4</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" ref="G28:I28" si="19">G12/$C$18</f>
+        <v>7.683073229291717E-3</v>
+      </c>
+      <c r="H28" s="9">
+        <f t="shared" si="19"/>
+        <v>5.7623049219687871E-3</v>
+      </c>
+      <c r="I28" s="9">
+        <f t="shared" si="19"/>
+        <v>1.4405762304921968E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F29" s="3">
+        <v>5</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" ref="G29:I29" si="20">G13/$C$18</f>
+        <v>3.2412965186074429E-3</v>
+      </c>
+      <c r="H29" s="9">
+        <f t="shared" si="20"/>
+        <v>3.2412965186074429E-3</v>
+      </c>
+      <c r="I29" s="9">
+        <f t="shared" si="20"/>
+        <v>1.0804321728691477E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F30" s="3">
+        <v>6</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" ref="G30:I30" si="21">G14/$C$18</f>
+        <v>9.6038415366146463E-4</v>
+      </c>
+      <c r="H30" s="9">
+        <f t="shared" si="21"/>
+        <v>1.4405762304921968E-3</v>
+      </c>
+      <c r="I30" s="15">
+        <f t="shared" si="21"/>
+        <v>7.2028811524609839E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F31" s="3">
+        <v>7</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" ref="G31:I31" si="22">G15/$C$18</f>
+        <v>9.6038415366146463E-4</v>
+      </c>
+      <c r="H31" s="9">
+        <f t="shared" si="22"/>
+        <v>1.4405762304921968E-3</v>
+      </c>
+      <c r="I31" s="15">
+        <f t="shared" si="22"/>
+        <v>7.2028811524609839E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F32" s="2">
+        <v>8</v>
+      </c>
+      <c r="G32" s="15">
+        <f t="shared" ref="G32:I32" si="23">G16/$C$18</f>
+        <v>1.2004801920768308E-4</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="G22:I22"/>
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="M20:P20"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="M6:P6"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1259,7 +1449,7 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <Ts>
-  <T C="16777215" N="List1" G="" P="False" K="ab5ebb93-d8c0-4754-a6ce-18d381e1d378:2038863848880" T="Worksheet" PI="0" L="" D="" A="638902842622800654" I="1"/>
+  <T C="16777215" N="List1" G="" P="False" K="ab5ebb93-d8c0-4754-a6ce-18d381e1d378:2465763803216" T="Worksheet" PI="0" L="" D="" A="638902925513764466" I="1"/>
 </Ts>
 </file>
 
@@ -1288,37 +1478,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1F5B93B-86BC-493E-A5F8-A27571E42EC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{329B7398-CB33-4C0D-BC1A-9E62EB4E0CFA}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A176A64-3F7F-497E-B9F8-E18D1034DE48}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BFC248-9FC8-40BF-996E-551CBB6DF1C3}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42ED8719-FBBB-486B-A595-4EC3022B9E90}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29FDE9FA-89F0-4CCB-88A5-BB6E4AF73B2C}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15932BC9-FC0D-4A5F-8E57-FF2AFF3F7681}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42841C43-5760-4F77-AB07-DC6E8BE887E8}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9B7B2C6-1D71-4990-B0AA-EA8E584E0C84}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D76BC3-98A6-4D47-A0B4-DE852D1532C5}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{213257A7-492E-4EF7-BEC2-1C39FA395526}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983ED0DE-2AEB-4EEB-8FA8-F07D973F3FC5}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>